<commit_message>
GFG-Add 1 to a number in the linked List
Question-Add 1 to a number in the linked List?
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EF237AF-442B-4813-AB03-2DF3ADD8D084}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C408D41-54AA-40E6-B674-790A89351F1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -37,6 +37,12 @@
   </si>
   <si>
     <t>Given head, the head of a linked list, determine if the linked list has a cycle in it.There is a cycle in a linked list if there is some node in the list that can be reached again by continuously following the next pointer. Internally, pos is used to denote the index of the node that tail's next pointer is connected to. Note that pos is not passed as a parameter.Return true if there is a cycle in the linked list. Otherwise, return false</t>
+  </si>
+  <si>
+    <t>Add 1 to a number represented as linked list</t>
+  </si>
+  <si>
+    <t>GFG</t>
   </si>
 </sst>
 </file>
@@ -374,10 +380,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,6 +416,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Reverse Nodes in k-Group
Same GFG and Leetcode problem but with slight variations
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C408D41-54AA-40E6-B674-790A89351F1E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F83D93C-E8CF-4D48-8D3B-ABB3D17EE151}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>GFG</t>
+  </si>
+  <si>
+    <t>Reverse Nodes in k-Group</t>
   </si>
 </sst>
 </file>
@@ -86,7 +89,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -99,6 +102,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -380,11 +386,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -392,7 +396,7 @@
     <col min="2" max="2" width="50.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -422,6 +426,14 @@
       </c>
       <c r="B4" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GFG-Intersection of Two sorted linked list
GFG-Intersection of Two sorted linked list
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1400CF-4332-4266-A5C6-96238E5F6997}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA52D679-9208-4A3C-B354-859463B0C950}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -61,6 +61,9 @@
   </si>
   <si>
     <t>Write a Program to Move the last element to Front in a Linked List.</t>
+  </si>
+  <si>
+    <t>Intersection of two sorted Linked lists</t>
   </si>
 </sst>
 </file>
@@ -404,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,6 +499,14 @@
         <v>11</v>
       </c>
     </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
876-Find Middle of the Linked List
876-Find Middle of the Linked List
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA52D679-9208-4A3C-B354-859463B0C950}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79694F8-5949-4AD3-8E2A-6A4163CE35A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Intersection of two sorted Linked lists</t>
+  </si>
+  <si>
+    <t>Middle of the Linked List</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -126,6 +129,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -407,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,6 +513,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>876</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG-Check If Circular Linked List
GFG-Check If Circular Linked List
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C79694F8-5949-4AD3-8E2A-6A4163CE35A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5812B378-1791-44BF-B95E-DD2F247F150D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Middle of the Linked List</t>
+  </si>
+  <si>
+    <t>Check If Circular Linked List</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +524,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG-Split a circular linked list into two halves
GFG-Split a circular linked list into two halves
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5812B378-1791-44BF-B95E-DD2F247F150D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F327AA41-5366-465C-9A4E-E9713249C07F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -70,6 +70,9 @@
   </si>
   <si>
     <t>Check If Circular Linked List</t>
+  </si>
+  <si>
+    <t>Split a Circular Linked List into two halves</t>
   </si>
 </sst>
 </file>
@@ -113,11 +116,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -131,10 +131,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -416,39 +416,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="50.140625" customWidth="1"/>
+    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="2" max="2" width="101.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>61</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:2" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>141</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -456,39 +456,39 @@
       <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>82</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>83</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>142</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -496,11 +496,11 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -517,7 +517,7 @@
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
+      <c r="A12" s="5">
         <v>876</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -530,6 +530,14 @@
       </c>
       <c r="B13" s="6" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
234.Palindrome of the Linked List
234.Palindrome of the Linked List
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F327AA41-5366-465C-9A4E-E9713249C07F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D097628-B49E-4A18-B26D-1070F247002F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>Split a Circular Linked List into two halves</t>
+  </si>
+  <si>
+    <t>Palindrome Linked List</t>
+  </si>
+  <si>
+    <t>GFG/234</t>
   </si>
 </sst>
 </file>
@@ -416,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,6 +546,14 @@
         <v>15</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Two Numbers GFG and Leetcode problem
Same problem but with slight variation in the inputs
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D097628-B49E-4A18-B26D-1070F247002F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4480E7-F57A-49F9-999B-BDC0E0338FB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -79,6 +79,12 @@
   </si>
   <si>
     <t>GFG/234</t>
+  </si>
+  <si>
+    <t>Add Two Numbers</t>
+  </si>
+  <si>
+    <t>Add Two Numbers(Non-reversed)-variation of Leetcode problem-2</t>
   </si>
 </sst>
 </file>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,6 +560,22 @@
         <v>16</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>2</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG-Merge Sort for Linked List
GFG-Merge Sort for Linked List
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4480E7-F57A-49F9-999B-BDC0E0338FB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C171B1-B2BA-4D1A-9609-8B46A0F66A4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Add Two Numbers(Non-reversed)-variation of Leetcode problem-2</t>
+  </si>
+  <si>
+    <t>Merge Sort For Linked lists.[Very Important]</t>
   </si>
 </sst>
 </file>
@@ -428,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,6 +579,14 @@
         <v>19</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG-Deletion from a Circular Linked List
GFG-Deletion from a Circular Linked List
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C171B1-B2BA-4D1A-9609-8B46A0F66A4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960BC3E9-4D8F-4BEE-9262-1F4F377018BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -88,6 +88,9 @@
   </si>
   <si>
     <t>Merge Sort For Linked lists.[Very Important]</t>
+  </si>
+  <si>
+    <t>Deletion from a Circular Linked List</t>
   </si>
 </sst>
 </file>
@@ -431,10 +434,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,6 +590,14 @@
         <v>20</v>
       </c>
     </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
24.GFG-Swap two nodes in pair
24.GFG-Swap two nodes in pair
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\Leetcode\Linked_List\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{960BC3E9-4D8F-4BEE-9262-1F4F377018BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77227758-F63C-4F15-8F69-6ACA302E12F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -91,6 +91,12 @@
   </si>
   <si>
     <t>Deletion from a Circular Linked List</t>
+  </si>
+  <si>
+    <t>24/GFG</t>
+  </si>
+  <si>
+    <t>Swap Nodes in Pairs</t>
   </si>
 </sst>
 </file>
@@ -434,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,6 +604,14 @@
         <v>21</v>
       </c>
     </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
1721.Swapping a node in a linked list
1721.Swapping a node in a linked list
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77227758-F63C-4F15-8F69-6ACA302E12F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3147C068-B4C9-4AB2-8D4B-A8B7B2CE23A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Swap Nodes in Pairs</t>
+  </si>
+  <si>
+    <t>Swapping Nodes in a Linked List</t>
   </si>
 </sst>
 </file>
@@ -440,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="G9" activeCellId="1" sqref="B21 G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,6 +615,14 @@
         <v>23</v>
       </c>
     </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>1721</v>
+      </c>
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
328-Odd and Even segregation of linked list
328-Odd and Even segregation of linked list
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3147C068-B4C9-4AB2-8D4B-A8B7B2CE23A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E980C2D4-B2C1-471D-8900-3E3A85B78C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Swapping Nodes in a Linked List</t>
+  </si>
+  <si>
+    <t>328/GFG</t>
+  </si>
+  <si>
+    <t>Odd Even Linked List</t>
   </si>
 </sst>
 </file>
@@ -443,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G9" activeCellId="1" sqref="B21 G9"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,6 +629,14 @@
         <v>24</v>
       </c>
     </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
GFG-Segregate even and odd nodes in a Linked List
GFG-Segregate even and odd nodes in a Linked List
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E980C2D4-B2C1-471D-8900-3E3A85B78C7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF7EE40-1185-4A96-831E-80017FB868F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Odd Even Linked List</t>
+  </si>
+  <si>
+    <t>Segregate even and odd nodes in a Link List </t>
   </si>
 </sst>
 </file>
@@ -449,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -637,6 +640,14 @@
         <v>26</v>
       </c>
     </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add Two Numbers(reverse and non-reversed)
Add Two Numbers(reverse and non-reversed)
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\Desktop\P_GIT\2022\Linked_List\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAF06F02-56A1-4635-96A7-528FB6D4804F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50054578-B0B0-4C51-B19F-9878FB9465FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Reverse Linked List II</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Java,Python</t>
   </si>
 </sst>
 </file>
@@ -458,27 +464,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="101.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>61</v>
       </c>
@@ -486,7 +496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>141</v>
       </c>
@@ -494,7 +504,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -502,7 +512,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>25</v>
       </c>
@@ -510,7 +520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>82</v>
       </c>
@@ -518,7 +528,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>83</v>
       </c>
@@ -526,7 +536,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>142</v>
       </c>
@@ -534,7 +544,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -542,7 +552,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -550,7 +560,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -558,7 +568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>876</v>
       </c>
@@ -566,7 +576,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -574,7 +584,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -582,7 +592,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -590,23 +600,29 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>2</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -614,7 +630,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -622,7 +638,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -630,7 +646,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>1721</v>
       </c>
@@ -638,7 +654,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
@@ -646,7 +662,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>5</v>
       </c>
@@ -654,7 +670,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
         <v>82</v>
       </c>
@@ -662,7 +678,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
         <v>92</v>
       </c>

</xml_diff>

<commit_message>
876. Middle of linked List- Java
876. Middle of linked List- Java
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50054578-B0B0-4C51-B19F-9878FB9465FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F43C75-F23C-4E2E-9E60-2217262BF23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -164,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -183,6 +183,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,25 +469,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
     <col min="2" max="2" width="101.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>30</v>
       </c>
     </row>
@@ -574,6 +577,9 @@
       </c>
       <c r="B12" s="6" t="s">
         <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
160. Intersection of Two Linked List- Java and Python
160. Intersection of Two Linked List- Java and Python
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F43C75-F23C-4E2E-9E60-2217262BF23B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8848777C-06ED-4D14-AD22-98B2990D2C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -121,6 +121,9 @@
   </si>
   <si>
     <t>Java,Python</t>
+  </si>
+  <si>
+    <t>Intersection of Two Linked Lists</t>
   </si>
 </sst>
 </file>
@@ -467,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,6 +695,17 @@
         <v>29</v>
       </c>
     </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>160</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Java version- Split a Circular Linked List into two halves
Java version- Split a Circular Linked List into two halves
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8848777C-06ED-4D14-AD22-98B2990D2C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECF52DD-7622-4495-AF08-B8F6B0F97220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -472,8 +472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,6 +600,9 @@
       <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">

</xml_diff>

<commit_message>
Java-Intersection Point in Y Shaped Linked Lists
Java-Intersection Point in Y Shaped Linked Lists
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ECF52DD-7622-4495-AF08-B8F6B0F97220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE28F53-33FC-48A3-9B21-548B42DE1A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>Intersection of Two Linked Lists</t>
+  </si>
+  <si>
+    <t>Intersection Point in Y Shaped Linked Lists</t>
+  </si>
+  <si>
+    <t>Java</t>
   </si>
 </sst>
 </file>
@@ -470,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,6 +715,17 @@
         <v>31</v>
       </c>
     </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Linked List question from strivers sheet
Linked List question from strivers sheet
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A287A2E3-9063-40C0-951D-7C135F18B0EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAA6457-53CE-4C2A-87AF-4D537424F136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Coding Ninja</t>
+  </si>
+  <si>
+    <t>Java/Python</t>
+  </si>
+  <si>
+    <t>Find length of Loop</t>
   </si>
 </sst>
 </file>
@@ -179,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -200,6 +206,9 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -482,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B29" sqref="A29:B29"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -521,6 +530,9 @@
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="C3" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -561,6 +573,9 @@
       <c r="B8" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="C8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -623,6 +638,9 @@
       <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
@@ -740,6 +758,17 @@
         <v>35</v>
       </c>
       <c r="C28" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
328. Odd Even Linked List
328. Odd Even Linked List -> Java solution
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAA6457-53CE-4C2A-87AF-4D537424F136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97944D3C-C87F-4BEE-9D9A-FC3814CB4C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Swapping Nodes in a Linked List</t>
   </si>
   <si>
-    <t>328/GFG</t>
-  </si>
-  <si>
     <t>Odd Even Linked List</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>Find length of Loop</t>
+  </si>
+  <si>
+    <t>Python</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -512,7 +512,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -531,7 +531,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -574,7 +574,7 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -609,7 +609,7 @@
         <v>13</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
         <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -639,7 +639,7 @@
         <v>16</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -650,7 +650,7 @@
         <v>18</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -661,7 +661,7 @@
         <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -697,11 +697,14 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="A22" s="5">
+        <v>328</v>
+      </c>
+      <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="B22" t="s">
-        <v>26</v>
+      <c r="C22" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -709,7 +712,10 @@
         <v>5</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -717,7 +723,7 @@
         <v>82</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -725,7 +731,7 @@
         <v>92</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
@@ -733,10 +739,10 @@
         <v>160</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -744,21 +750,21 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C27" t="s">
         <v>33</v>
-      </c>
-      <c r="C27" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -766,10 +772,10 @@
         <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
LC-19 and GFG. Nth node from end of linked list.
LC-19 and GFG. Nth node from end of linked list.
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97944D3C-C87F-4BEE-9D9A-FC3814CB4C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B65EAF-F273-4D91-9ADE-EB6D0BD6BC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>Python</t>
+  </si>
+  <si>
+    <t>Remove Nth Node From End of List</t>
+  </si>
+  <si>
+    <t>Nth node from end of linked list</t>
   </si>
 </sst>
 </file>
@@ -185,14 +191,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -210,6 +210,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -491,86 +500,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" style="8" customWidth="1"/>
     <col min="2" max="2" width="101.85546875" customWidth="1"/>
     <col min="3" max="3" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="8">
         <v>61</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="8">
         <v>141</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4" t="s">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="9">
         <v>25</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="9">
         <v>82</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="9">
         <v>83</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="9">
         <v>142</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
@@ -578,34 +587,34 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="6" t="s">
+      <c r="A10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="6" t="s">
+      <c r="A11" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+      <c r="A12" s="8">
         <v>876</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C12" t="s">
@@ -613,18 +622,18 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="6" t="s">
+      <c r="A13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="6" t="s">
+      <c r="A14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C14" t="s">
@@ -632,10 +641,10 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C15" t="s">
@@ -643,10 +652,10 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="6">
+      <c r="A16" s="9">
         <v>2</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C16" t="s">
@@ -654,10 +663,10 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C17" t="s">
@@ -665,7 +674,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B18" t="s">
@@ -673,7 +682,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="A19" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B19" t="s">
@@ -681,7 +690,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="8" t="s">
         <v>22</v>
       </c>
       <c r="B20" t="s">
@@ -689,7 +698,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
+      <c r="A21" s="8">
         <v>1721</v>
       </c>
       <c r="B21" t="s">
@@ -697,7 +706,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+      <c r="A22" s="8">
         <v>328</v>
       </c>
       <c r="B22" t="s">
@@ -708,10 +717,10 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="6" t="s">
+      <c r="A23" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C23" t="s">
@@ -719,23 +728,23 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+      <c r="A24" s="8">
         <v>82</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="5">
+      <c r="A25" s="8">
         <v>92</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="8">
         <v>160</v>
       </c>
       <c r="B26" t="s">
@@ -746,7 +755,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B27" t="s">
@@ -757,7 +766,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="A28" s="8" t="s">
         <v>35</v>
       </c>
       <c r="B28" t="s">
@@ -768,7 +777,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+      <c r="A29" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B29" t="s">
@@ -776,6 +785,28 @@
       </c>
       <c r="C29" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>19</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" t="s">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
148. Sort List and 2095. Delete the middle Node of linked list
148. Sort List and 2095. Delete the middle Node of linked list
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5B65EAF-F273-4D91-9ADE-EB6D0BD6BC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EABC7D-6499-447E-B7E9-AEBEA1C85ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Nth node from end of linked list</t>
+  </si>
+  <si>
+    <t>Delete the Middle Node of a Linked List</t>
+  </si>
+  <si>
+    <t>Sort List</t>
   </si>
 </sst>
 </file>
@@ -500,10 +506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,6 +815,28 @@
         <v>36</v>
       </c>
     </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>2095</v>
+      </c>
+      <c r="B32" t="s">
+        <v>41</v>
+      </c>
+      <c r="C32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>148</v>
+      </c>
+      <c r="B33" t="s">
+        <v>42</v>
+      </c>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B28" r:id="rId1" display="https://www.geeksforgeeks.org/move-last-element-to-front-of-a-given-linked-list/" xr:uid="{E24E1B1E-D4E4-4B06-9E99-5290A9E89D36}"/>

</xml_diff>

<commit_message>
GFG. Given a linked list of 0s, 1s and 2s, sort it
GFG. Given a linked list of 0s, 1s and 2s, sort it
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6EABC7D-6499-447E-B7E9-AEBEA1C85ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19C1C7C-AA2B-4E89-8FEF-08A5B69D46C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Sort List</t>
+  </si>
+  <si>
+    <t>Given a linked list of 0s, 1s and 2s, sort it.</t>
   </si>
 </sst>
 </file>
@@ -506,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -837,6 +840,17 @@
         <v>33</v>
       </c>
     </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B28" r:id="rId1" display="https://www.geeksforgeeks.org/move-last-element-to-front-of-a-given-linked-list/" xr:uid="{E24E1B1E-D4E4-4B06-9E99-5290A9E89D36}"/>

</xml_diff>

<commit_message>
GFG. Add 1 to a number represented as linked list
GFG. Add 1 to a number represented as linked list
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19C1C7C-AA2B-4E89-8FEF-08A5B69D46C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614EB6EA-A572-4913-9954-E8EFBFF4C968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -511,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,6 +559,9 @@
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="9">

</xml_diff>

<commit_message>
61. Rotate a Linked List and its variation
61. Rotate a Linked List and its variation
GFG. Doubly LL target problem
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614EB6EA-A572-4913-9954-E8EFBFF4C968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C54BE04-9AAD-45C1-86BE-D8E614FE7A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>Given a linked list of 0s, 1s and 2s, sort it.</t>
+  </si>
+  <si>
+    <t>Find pairs with given sum in doubly linked list</t>
   </si>
 </sst>
 </file>
@@ -180,12 +183,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -200,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -228,6 +237,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -509,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -534,11 +559,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="8">
+      <c r="A2" s="10">
         <v>61</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="11" t="s">
         <v>2</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -553,21 +581,21 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="12" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
+    <row r="5" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13">
         <v>25</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="14" t="s">
         <v>6</v>
       </c>
     </row>
@@ -614,22 +642,22 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="4" t="s">
+    <row r="11" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="8">
+    <row r="12" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
         <v>876</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="12" t="s">
         <v>30</v>
       </c>
     </row>
@@ -663,25 +691,25 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="9">
+    <row r="16" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13">
         <v>2</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="12" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="12" t="s">
         <v>30</v>
       </c>
     </row>
@@ -717,14 +745,14 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="8">
+    <row r="22" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
         <v>328</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="12" t="s">
         <v>36</v>
       </c>
     </row>
@@ -822,35 +850,46 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="8">
+      <c r="A32" s="10">
         <v>2095</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="8">
+      <c r="A33" s="10">
         <v>148</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="12" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="A34" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" s="12" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1 GFG problem on LL and Doubly Linked List
1 GFG problem on LL and Doubly Linked List
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C54BE04-9AAD-45C1-86BE-D8E614FE7A90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C98546-CEF7-4900-A2C0-72BC405C1AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -160,6 +160,12 @@
   </si>
   <si>
     <t>Find pairs with given sum in doubly linked list</t>
+  </si>
+  <si>
+    <t>Flattening a Linked List</t>
+  </si>
+  <si>
+    <t>Remove duplicates from a sorted doubly linked list</t>
   </si>
 </sst>
 </file>
@@ -534,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C35"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,6 +899,28 @@
         <v>33</v>
       </c>
     </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B28" r:id="rId1" display="https://www.geeksforgeeks.org/move-last-element-to-front-of-a-given-linked-list/" xr:uid="{E24E1B1E-D4E4-4B06-9E99-5290A9E89D36}"/>

</xml_diff>

<commit_message>
Updated and add new Problem on DLL and LL
Updated and add new Problem on DLL and LL
</commit_message>
<xml_diff>
--- a/Linked_List/Question_Linked_List.xlsx
+++ b/Linked_List/Question_Linked_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pnaik27\OneDrive - DXC Production\Desktop\Personal_git\Leetcode\Linked_List\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C98546-CEF7-4900-A2C0-72BC405C1AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{797124D8-A5F3-432E-A642-3542F01F62D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
   <si>
     <t>Leetcode Question No.</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>Remove duplicates from a sorted doubly linked list</t>
+  </si>
+  <si>
+    <t>Delete all occurrences of a given key in a doubly linked list</t>
   </si>
 </sst>
 </file>
@@ -540,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,7 +567,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>61</v>
       </c>
@@ -586,7 +589,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>5</v>
       </c>
@@ -918,6 +921,28 @@
         <v>46</v>
       </c>
       <c r="C37" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="12" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>